<commit_message>
made the parallel thing
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="sequential" sheetId="1" r:id="rId1"/>
+    <sheet name="parallel" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>Subjects</t>
   </si>
@@ -24,16 +24,7 @@
     <t>target</t>
   </si>
   <si>
-    <t>Found?</t>
-  </si>
-  <si>
     <t>Time(NanoSeconds)</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -365,18 +356,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,64 +377,60 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="C2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
-        <v>40000</v>
+        <v>100</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>25315</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="C3">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
-        <v>40000</v>
+        <v>1000</v>
       </c>
       <c r="B4">
-        <v>200</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>12245623</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>11109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
-        <v>40000</v>
+        <v>10000</v>
       </c>
       <c r="B5">
-        <v>200</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>12272320</v>
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>977719</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>100000</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>95578030</v>
       </c>
     </row>
   </sheetData>
@@ -453,12 +440,66 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>1000</v>
+      </c>
+      <c r="B4">
+        <v>11250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>10000</v>
+      </c>
+      <c r="B5">
+        <v>974163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>100000</v>
+      </c>
+      <c r="B6">
+        <v>95233035</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>